<commit_message>
Updated project management spreadsheet
</commit_message>
<xml_diff>
--- a/team_folder/newFolder/Project Management.xlsx
+++ b/team_folder/newFolder/Project Management.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Leads and Support" sheetId="1" state="visible" r:id="rId2"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="123">
   <si>
     <t xml:space="preserve">newFolder</t>
   </si>
@@ -206,10 +206,13 @@
     <t xml:space="preserve">Create a block diagram for PWM</t>
   </si>
   <si>
-    <t xml:space="preserve">Python Motor design (pseudo code/examples/diagrams)</t>
+    <t xml:space="preserve">Python Motor idea implementation</t>
   </si>
   <si>
     <t xml:space="preserve">Wrapped memory access logic in class – modularization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Python Sensor idea implementation</t>
   </si>
   <si>
     <t xml:space="preserve">Explore opencv object detection</t>
@@ -840,7 +843,7 @@
   </sheetPr>
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -849,7 +852,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="31.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="31.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.86"/>
@@ -1043,7 +1046,7 @@
   </sheetPr>
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I24" activeCellId="0" sqref="I24"/>
     </sheetView>
   </sheetViews>
@@ -1558,8 +1561,8 @@
   </sheetPr>
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J12" activeCellId="0" sqref="J12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1568,8 +1571,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.73"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.73"/>
@@ -1894,7 +1897,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="24" t="n">
-        <v>43164</v>
+        <v>43160</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>60</v>
@@ -1911,26 +1914,21 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="15" t="n">
-        <v>43165</v>
+      <c r="A15" s="24" t="n">
+        <v>43164</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>61</v>
       </c>
       <c r="C15" s="23" t="n">
-        <v>2</v>
-      </c>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
+        <v>1</v>
+      </c>
       <c r="I15" s="23" t="n">
         <v>1</v>
       </c>
       <c r="J15" s="23" t="n">
         <f aca="false">SUM(D15:I15)*$M$1*C15</f>
-        <v>200</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1938,28 +1936,38 @@
         <v>43165</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="C16" s="23"/>
+        <v>62</v>
+      </c>
+      <c r="C16" s="23" t="n">
+        <v>2</v>
+      </c>
       <c r="D16" s="23"/>
       <c r="E16" s="23"/>
       <c r="F16" s="23"/>
-      <c r="G16" s="23" t="n">
-        <v>1</v>
-      </c>
+      <c r="G16" s="23"/>
       <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
+      <c r="I16" s="23" t="n">
+        <v>1</v>
+      </c>
       <c r="J16" s="23" t="n">
         <f aca="false">SUM(D16:I16)*$M$1*C16</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="15" t="n">
+        <v>43165</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>56</v>
+      </c>
       <c r="C17" s="23"/>
       <c r="D17" s="23"/>
       <c r="E17" s="23"/>
       <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
+      <c r="G17" s="23" t="n">
+        <v>1</v>
+      </c>
       <c r="H17" s="23"/>
       <c r="I17" s="23"/>
       <c r="J17" s="23" t="n">
@@ -2028,7 +2036,7 @@
       <c r="I23" s="23"/>
       <c r="J23" s="23" t="n">
         <f aca="false">SUM(J2:J22)</f>
-        <v>1450</v>
+        <v>1550</v>
       </c>
     </row>
   </sheetData>
@@ -2051,7 +2059,7 @@
   </sheetPr>
   <dimension ref="A1:P45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K17" activeCellId="0" sqref="K17"/>
     </sheetView>
   </sheetViews>
@@ -2060,9 +2068,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="41.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="5.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.72"/>
@@ -2078,7 +2086,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="25" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="25"/>
@@ -2092,50 +2100,50 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="28" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F2" s="30" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G2" s="30" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H2" s="31"/>
       <c r="I2" s="28" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J2" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="K2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="L2" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="M2" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="N2" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="O2" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="P2" s="30" t="s">
         <v>70</v>
-      </c>
-      <c r="K2" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="L2" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="M2" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="N2" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="O2" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="P2" s="30" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2157,7 +2165,7 @@
         <v>8</v>
       </c>
       <c r="G3" s="36" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H3" s="37"/>
       <c r="I3" s="38" t="n">
@@ -2167,7 +2175,7 @@
         <v>16</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="L3" s="23"/>
       <c r="M3" s="23" t="n">
@@ -2180,7 +2188,7 @@
         <v>8</v>
       </c>
       <c r="P3" s="23" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2200,7 +2208,7 @@
       </c>
       <c r="F4" s="35"/>
       <c r="G4" s="36" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H4" s="37"/>
       <c r="I4" s="38" t="n">
@@ -2208,7 +2216,7 @@
       </c>
       <c r="J4" s="38"/>
       <c r="K4" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="L4" s="23"/>
       <c r="M4" s="23" t="n">
@@ -2219,7 +2227,7 @@
         <v>8</v>
       </c>
       <c r="P4" s="23" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2241,14 +2249,14 @@
         <v>8</v>
       </c>
       <c r="G5" s="36" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H5" s="37"/>
       <c r="I5" s="38" t="n">
         <v>1.3</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L5" s="23"/>
       <c r="M5" s="23" t="n">
@@ -2259,7 +2267,7 @@
         <v>8</v>
       </c>
       <c r="P5" s="23" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2268,7 +2276,7 @@
         <v>1.4</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C6" s="32" t="n">
         <v>1</v>
@@ -2283,14 +2291,14 @@
         <v>40</v>
       </c>
       <c r="G6" s="36" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H6" s="37"/>
       <c r="I6" s="38" t="n">
         <v>1.4</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L6" s="23"/>
       <c r="M6" s="23" t="n">
@@ -2301,7 +2309,7 @@
         <v>8</v>
       </c>
       <c r="P6" s="39" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2310,7 +2318,7 @@
         <v>1.5</v>
       </c>
       <c r="B7" s="33" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C7" s="32" t="n">
         <v>1</v>
@@ -2325,14 +2333,14 @@
         <v>39</v>
       </c>
       <c r="G7" s="36" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H7" s="37"/>
       <c r="I7" s="38" t="n">
         <v>1.5</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="L7" s="23"/>
       <c r="M7" s="23" t="n">
@@ -2340,10 +2348,10 @@
       </c>
       <c r="N7" s="23"/>
       <c r="O7" s="23" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="P7" s="23" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2352,7 +2360,7 @@
         <v>1.6</v>
       </c>
       <c r="B8" s="33" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C8" s="32" t="n">
         <v>1</v>
@@ -2367,7 +2375,7 @@
         <v>9</v>
       </c>
       <c r="G8" s="36" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H8" s="37"/>
       <c r="I8" s="38" t="n">
@@ -2380,7 +2388,7 @@
         <v>1.7</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C9" s="32" t="n">
         <v>1</v>
@@ -2395,7 +2403,7 @@
         <v>23</v>
       </c>
       <c r="G9" s="36" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H9" s="37"/>
       <c r="I9" s="38" t="n">
@@ -2408,7 +2416,7 @@
         <v>1.8</v>
       </c>
       <c r="B10" s="33" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C10" s="32" t="n">
         <v>1</v>
@@ -2423,7 +2431,7 @@
         <v>34</v>
       </c>
       <c r="G10" s="36" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H10" s="37"/>
       <c r="J10" s="23" t="s">
@@ -2436,7 +2444,7 @@
         <v>1.9</v>
       </c>
       <c r="B11" s="33" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C11" s="32" t="n">
         <v>1</v>
@@ -2451,14 +2459,14 @@
         <v>8</v>
       </c>
       <c r="G11" s="36" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H11" s="37"/>
       <c r="I11" s="23" t="n">
         <v>2.1</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="L11" s="23"/>
       <c r="M11" s="40" t="n">
@@ -2469,7 +2477,7 @@
         <v>34</v>
       </c>
       <c r="P11" s="38" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2488,7 +2496,7 @@
       <c r="M12" s="23"/>
       <c r="N12" s="23"/>
       <c r="O12" s="23" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="P12" s="23"/>
     </row>
@@ -2501,7 +2509,7 @@
         <v>2.3</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="L13" s="0" t="n">
         <v>1</v>
@@ -2516,7 +2524,7 @@
         <v>39</v>
       </c>
       <c r="P13" s="23" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2525,7 +2533,7 @@
         <v>1.12</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>3</v>
@@ -2534,13 +2542,13 @@
         <v>34</v>
       </c>
       <c r="G14" s="37" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I14" s="23" t="n">
         <v>2.4</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="L14" s="23"/>
       <c r="M14" s="23" t="n">
@@ -2548,10 +2556,10 @@
       </c>
       <c r="N14" s="23"/>
       <c r="O14" s="37" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="P14" s="39" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2563,7 +2571,7 @@
         <v>2.5</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="L15" s="23"/>
       <c r="M15" s="23"/>
@@ -2580,7 +2588,7 @@
         <v>2.6</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="L16" s="23"/>
       <c r="M16" s="23" t="n">
@@ -2588,10 +2596,10 @@
       </c>
       <c r="N16" s="23"/>
       <c r="O16" s="37" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="P16" s="39" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2603,7 +2611,7 @@
         <v>2.7</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L17" s="23"/>
       <c r="M17" s="23" t="n">
@@ -2611,10 +2619,10 @@
       </c>
       <c r="N17" s="23"/>
       <c r="O17" s="37" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="P17" s="39" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2624,7 +2632,7 @@
       </c>
       <c r="I18" s="23"/>
       <c r="K18" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="L18" s="23"/>
       <c r="M18" s="23" t="n">
@@ -2632,10 +2640,10 @@
       </c>
       <c r="N18" s="23"/>
       <c r="O18" s="37" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="P18" s="37" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2656,7 +2664,7 @@
       <c r="M19" s="23"/>
       <c r="N19" s="23"/>
       <c r="O19" s="37" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P19" s="23"/>
     </row>
@@ -2669,13 +2677,13 @@
         <v>3.2</v>
       </c>
       <c r="K20" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="L20" s="23"/>
       <c r="M20" s="23"/>
       <c r="N20" s="23"/>
       <c r="O20" s="23" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="P20" s="23"/>
     </row>
@@ -2688,7 +2696,7 @@
         <v>3.3</v>
       </c>
       <c r="K21" s="7" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="L21" s="23"/>
       <c r="M21" s="23" t="n">
@@ -2696,10 +2704,10 @@
       </c>
       <c r="N21" s="23"/>
       <c r="O21" s="37" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P21" s="37" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2711,13 +2719,13 @@
         <v>3.4</v>
       </c>
       <c r="K22" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="L22" s="23"/>
       <c r="M22" s="23"/>
       <c r="N22" s="23"/>
       <c r="O22" s="37" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P22" s="23"/>
     </row>
@@ -2730,7 +2738,7 @@
         <v>3.5</v>
       </c>
       <c r="K23" s="7" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="L23" s="23"/>
       <c r="M23" s="23" t="n">
@@ -2738,10 +2746,10 @@
       </c>
       <c r="N23" s="23"/>
       <c r="O23" s="37" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P23" s="39" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2753,7 +2761,7 @@
         <v>3.6</v>
       </c>
       <c r="K24" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="L24" s="23"/>
       <c r="M24" s="23" t="n">
@@ -2761,10 +2769,10 @@
       </c>
       <c r="N24" s="23"/>
       <c r="O24" s="37" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P24" s="39" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2776,13 +2784,13 @@
         <v>3.7</v>
       </c>
       <c r="K25" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="L25" s="23"/>
       <c r="M25" s="23"/>
       <c r="N25" s="23"/>
       <c r="O25" s="37" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P25" s="23"/>
     </row>
@@ -2793,7 +2801,7 @@
         <v>3.8</v>
       </c>
       <c r="K26" s="7" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="L26" s="23"/>
       <c r="M26" s="23" t="n">
@@ -2801,10 +2809,10 @@
       </c>
       <c r="N26" s="23"/>
       <c r="O26" s="37" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="P26" s="37" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2820,10 +2828,10 @@
         <v>4.1</v>
       </c>
       <c r="J28" s="23" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="K28" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="L28" s="23"/>
       <c r="M28" s="23" t="n">
@@ -2831,7 +2839,7 @@
       </c>
       <c r="N28" s="23"/>
       <c r="O28" s="37" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="P28" s="23"/>
     </row>
@@ -2840,7 +2848,7 @@
         <v>4.2</v>
       </c>
       <c r="K29" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="L29" s="23"/>
       <c r="M29" s="23" t="n">
@@ -2848,10 +2856,10 @@
       </c>
       <c r="N29" s="23"/>
       <c r="O29" s="37" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="P29" s="39" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2859,7 +2867,7 @@
         <v>4.3</v>
       </c>
       <c r="K30" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="L30" s="23"/>
       <c r="M30" s="23" t="n">
@@ -2867,10 +2875,10 @@
       </c>
       <c r="N30" s="23"/>
       <c r="O30" s="37" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="P30" s="39" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2886,10 +2894,10 @@
         <v>5.1</v>
       </c>
       <c r="J32" s="23" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="K32" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="L32" s="23"/>
       <c r="M32" s="40" t="n">
@@ -2900,7 +2908,7 @@
         <v>34</v>
       </c>
       <c r="P32" s="38" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2908,7 +2916,7 @@
         <v>5.2</v>
       </c>
       <c r="K33" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="L33" s="23"/>
       <c r="M33" s="40" t="n">
@@ -2919,7 +2927,7 @@
         <v>34</v>
       </c>
       <c r="P33" s="38" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2927,7 +2935,7 @@
         <v>5.3</v>
       </c>
       <c r="K34" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="L34" s="23"/>
       <c r="M34" s="40" t="n">
@@ -2938,7 +2946,7 @@
         <v>34</v>
       </c>
       <c r="P34" s="38" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2946,7 +2954,7 @@
         <v>5.4</v>
       </c>
       <c r="K35" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="L35" s="23"/>
       <c r="M35" s="40" t="n">
@@ -2957,7 +2965,7 @@
         <v>34</v>
       </c>
       <c r="P35" s="38" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2965,7 +2973,7 @@
         <v>5.5</v>
       </c>
       <c r="K36" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L36" s="23"/>
       <c r="M36" s="40" t="n">
@@ -2976,15 +2984,15 @@
         <v>34</v>
       </c>
       <c r="P36" s="38" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J38" s="23" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="K38" s="33" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="L38" s="32" t="n">
         <v>1.5</v>
@@ -2996,10 +3004,10 @@
         <v>3</v>
       </c>
       <c r="O38" s="35" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="P38" s="36" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3014,40 +3022,40 @@
         <v>3</v>
       </c>
       <c r="O39" s="37" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="P39" s="23" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K40" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K41" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K42" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K43" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K44" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K45" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>